<commit_message>
Completed conversion of measurement system
Yet to check all changes have been implemented correctly.
</commit_message>
<xml_diff>
--- a/src/test/resources/images/BinarySphere3D_8bit1.xlsx
+++ b/src/test/resources/images/BinarySphere3D_8bit1.xlsx
@@ -8,7 +8,7 @@
   <sheets>
     <sheet name="Parameters" r:id="rId3" sheetId="1"/>
     <sheet name="Summary" r:id="rId4" sheetId="2"/>
-    <sheet name="OBJ_Ring" r:id="rId5" sheetId="3"/>
+    <sheet name="OBJ_Sphere" r:id="rId5" sheetId="3"/>
   </sheets>
 </workbook>
 </file>
@@ -339,7 +339,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>false</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -356,7 +356,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Rings</t>
+          <t>Shell</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -390,7 +390,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>E:\Stephen\Java Projects\ModularImageAnalysis\src\test\resources\images\MeasureObjectIntensity\BinarySphere3D_10pxOutsideShell_8bit.tif</t>
+          <t>C:\Users\steph\Documents\Java Projects\ModularImageAnalysis\src\test\resources\images\MeasureObjectIntensity\BinarySphere3D_10pxOutsideShell_8bit.tif</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -611,7 +611,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>false</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
@@ -645,7 +645,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Ring</t>
+          <t>Sphere</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
@@ -713,7 +713,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Ring</t>
+          <t>Sphere</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
@@ -730,7 +730,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Rings</t>
+          <t>Shell</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
@@ -986,1414 +986,1414 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>RING_(OBJ)//NUMBER</t>
+          <t>SPHERE_(OBJ)//NUMBER</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_MEAN</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_MEAN</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_MEAN</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_MEAN</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_MEAN</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_MEAN</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_MEAN</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_MEAN</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_MEAN</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_MEAN</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_MIN</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_MIN</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_MIN</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_MIN</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_MIN</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_MIN</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_MIN</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_MIN</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_MIN</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_MIN</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_MAX</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_MAX</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_MAX</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_MAX</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_MAX</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_MAX</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_MAX</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_MAX</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_MAX</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_MAX</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_STDEV</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_STDEV</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_STDEV</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_STDEV</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_STDEV</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_STDEV</t>
         </is>
       </c>
       <c r="V1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_STDEV</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_STDEV</t>
         </is>
       </c>
       <c r="W1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_STDEV</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_STDEV</t>
         </is>
       </c>
       <c r="X1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_SUM</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_SUM</t>
         </is>
       </c>
       <c r="Y1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_SUM</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_SUM</t>
         </is>
       </c>
       <c r="Z1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_SUM</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_SUM</t>
         </is>
       </c>
       <c r="AA1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_SUM</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_SUM</t>
         </is>
       </c>
       <c r="AB1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_SUM</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_SUM</t>
         </is>
       </c>
       <c r="AC1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_X_CENTRE_MEAN_(PX)</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_X_CENTRE_MEAN_(PX)</t>
         </is>
       </c>
       <c r="AD1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_X_CENTRE_MEAN_(PX)</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_X_CENTRE_MEAN_(PX)</t>
         </is>
       </c>
       <c r="AE1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_X_CENTRE_MEAN_(PX)</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_X_CENTRE_MEAN_(PX)</t>
         </is>
       </c>
       <c r="AF1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_X_CENTRE_MEAN_(PX)</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_X_CENTRE_MEAN_(PX)</t>
         </is>
       </c>
       <c r="AG1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_X_CENTRE_MEAN_(PX)</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_X_CENTRE_MEAN_(PX)</t>
         </is>
       </c>
       <c r="AH1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_X_CENTRE_STDEV_(PX)</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_X_CENTRE_STDEV_(PX)</t>
         </is>
       </c>
       <c r="AI1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_X_CENTRE_STDEV_(PX)</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_X_CENTRE_STDEV_(PX)</t>
         </is>
       </c>
       <c r="AJ1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_X_CENTRE_STDEV_(PX)</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_X_CENTRE_STDEV_(PX)</t>
         </is>
       </c>
       <c r="AK1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_X_CENTRE_STDEV_(PX)</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_X_CENTRE_STDEV_(PX)</t>
         </is>
       </c>
       <c r="AL1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_X_CENTRE_STDEV_(PX)</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_X_CENTRE_STDEV_(PX)</t>
         </is>
       </c>
       <c r="AM1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_Y_CENTRE_MEAN_(PX)</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_Y_CENTRE_MEAN_(PX)</t>
         </is>
       </c>
       <c r="AN1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_Y_CENTRE_MEAN_(PX)</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_Y_CENTRE_MEAN_(PX)</t>
         </is>
       </c>
       <c r="AO1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_Y_CENTRE_MEAN_(PX)</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_Y_CENTRE_MEAN_(PX)</t>
         </is>
       </c>
       <c r="AP1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_Y_CENTRE_MEAN_(PX)</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_Y_CENTRE_MEAN_(PX)</t>
         </is>
       </c>
       <c r="AQ1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_Y_CENTRE_MEAN_(PX)</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_Y_CENTRE_MEAN_(PX)</t>
         </is>
       </c>
       <c r="AR1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_Y_CENTRE_STDEV_(PX)</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_Y_CENTRE_STDEV_(PX)</t>
         </is>
       </c>
       <c r="AS1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_Y_CENTRE_STDEV_(PX)</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_Y_CENTRE_STDEV_(PX)</t>
         </is>
       </c>
       <c r="AT1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_Y_CENTRE_STDEV_(PX)</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_Y_CENTRE_STDEV_(PX)</t>
         </is>
       </c>
       <c r="AU1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_Y_CENTRE_STDEV_(PX)</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_Y_CENTRE_STDEV_(PX)</t>
         </is>
       </c>
       <c r="AV1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_Y_CENTRE_STDEV_(PX)</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_Y_CENTRE_STDEV_(PX)</t>
         </is>
       </c>
       <c r="AW1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_Z_CENTRE_MEAN_(SLICE)</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_Z_CENTRE_MEAN_(SLICE)</t>
         </is>
       </c>
       <c r="AX1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_Z_CENTRE_MEAN_(SLICE)</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_Z_CENTRE_MEAN_(SLICE)</t>
         </is>
       </c>
       <c r="AY1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_Z_CENTRE_MEAN_(SLICE)</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_Z_CENTRE_MEAN_(SLICE)</t>
         </is>
       </c>
       <c r="AZ1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_Z_CENTRE_MEAN_(SLICE)</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_Z_CENTRE_MEAN_(SLICE)</t>
         </is>
       </c>
       <c r="BA1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_Z_CENTRE_MEAN_(SLICE)</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_Z_CENTRE_MEAN_(SLICE)</t>
         </is>
       </c>
       <c r="BB1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_Z_CENTRE_STDEV_(SLICE)</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_Z_CENTRE_STDEV_(SLICE)</t>
         </is>
       </c>
       <c r="BC1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_Z_CENTRE_STDEV_(SLICE)</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_Z_CENTRE_STDEV_(SLICE)</t>
         </is>
       </c>
       <c r="BD1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_Z_CENTRE_STDEV_(SLICE)</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_Z_CENTRE_STDEV_(SLICE)</t>
         </is>
       </c>
       <c r="BE1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_Z_CENTRE_STDEV_(SLICE)</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_Z_CENTRE_STDEV_(SLICE)</t>
         </is>
       </c>
       <c r="BF1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_Z_CENTRE_STDEV_(SLICE)</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_Z_CENTRE_STDEV_(SLICE)</t>
         </is>
       </c>
       <c r="BG1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_MEAN_EDGE_DISTANCE_(PX)</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_MEAN_EDGE_DISTANCE_(PX)</t>
         </is>
       </c>
       <c r="BH1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_MEAN_EDGE_DISTANCE_(PX)</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_MEAN_EDGE_DISTANCE_(PX)</t>
         </is>
       </c>
       <c r="BI1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_MEAN_EDGE_DISTANCE_(PX)</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_MEAN_EDGE_DISTANCE_(PX)</t>
         </is>
       </c>
       <c r="BJ1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_MEAN_EDGE_DISTANCE_(PX)</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_MEAN_EDGE_DISTANCE_(PX)</t>
         </is>
       </c>
       <c r="BK1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_MEAN_EDGE_DISTANCE_(PX)</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_MEAN_EDGE_DISTANCE_(PX)</t>
         </is>
       </c>
       <c r="BL1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_MEAN_EDGE_DISTANCE_(CAL)</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_MEAN_EDGE_DISTANCE_(CAL)</t>
         </is>
       </c>
       <c r="BM1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_MEAN_EDGE_DISTANCE_(CAL)</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_MEAN_EDGE_DISTANCE_(CAL)</t>
         </is>
       </c>
       <c r="BN1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_MEAN_EDGE_DISTANCE_(CAL)</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_MEAN_EDGE_DISTANCE_(CAL)</t>
         </is>
       </c>
       <c r="BO1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_MEAN_EDGE_DISTANCE_(CAL)</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_MEAN_EDGE_DISTANCE_(CAL)</t>
         </is>
       </c>
       <c r="BP1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_MEAN_EDGE_DISTANCE_(CAL)</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_MEAN_EDGE_DISTANCE_(CAL)</t>
         </is>
       </c>
       <c r="BQ1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_STD_EDGE_DISTANCE_(PX)</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_STD_EDGE_DISTANCE_(PX)</t>
         </is>
       </c>
       <c r="BR1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_STD_EDGE_DISTANCE_(PX)</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_STD_EDGE_DISTANCE_(PX)</t>
         </is>
       </c>
       <c r="BS1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_STD_EDGE_DISTANCE_(PX)</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_STD_EDGE_DISTANCE_(PX)</t>
         </is>
       </c>
       <c r="BT1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_STD_EDGE_DISTANCE_(PX)</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_STD_EDGE_DISTANCE_(PX)</t>
         </is>
       </c>
       <c r="BU1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_STD_EDGE_DISTANCE_(PX)</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_STD_EDGE_DISTANCE_(PX)</t>
         </is>
       </c>
       <c r="BV1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_STD_EDGE_DISTANCE_(CAL)</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_STD_EDGE_DISTANCE_(CAL)</t>
         </is>
       </c>
       <c r="BW1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_STD_EDGE_DISTANCE_(CAL)</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_STD_EDGE_DISTANCE_(CAL)</t>
         </is>
       </c>
       <c r="BX1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_STD_EDGE_DISTANCE_(CAL)</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_STD_EDGE_DISTANCE_(CAL)</t>
         </is>
       </c>
       <c r="BY1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_STD_EDGE_DISTANCE_(CAL)</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_STD_EDGE_DISTANCE_(CAL)</t>
         </is>
       </c>
       <c r="BZ1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_STD_EDGE_DISTANCE_(CAL)</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_STD_EDGE_DISTANCE_(CAL)</t>
         </is>
       </c>
       <c r="CA1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN1</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN1</t>
         </is>
       </c>
       <c r="CB1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN1</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN1</t>
         </is>
       </c>
       <c r="CC1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN1</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN1</t>
         </is>
       </c>
       <c r="CD1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN1</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN1</t>
         </is>
       </c>
       <c r="CE1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN1</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN1</t>
         </is>
       </c>
       <c r="CF1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN2</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN2</t>
         </is>
       </c>
       <c r="CG1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN2</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN2</t>
         </is>
       </c>
       <c r="CH1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN2</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN2</t>
         </is>
       </c>
       <c r="CI1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN2</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN2</t>
         </is>
       </c>
       <c r="CJ1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN2</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN2</t>
         </is>
       </c>
       <c r="CK1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN3</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN3</t>
         </is>
       </c>
       <c r="CL1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN3</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN3</t>
         </is>
       </c>
       <c r="CM1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN3</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN3</t>
         </is>
       </c>
       <c r="CN1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN3</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN3</t>
         </is>
       </c>
       <c r="CO1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN3</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN3</t>
         </is>
       </c>
       <c r="CP1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN4</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN4</t>
         </is>
       </c>
       <c r="CQ1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN4</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN4</t>
         </is>
       </c>
       <c r="CR1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN4</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN4</t>
         </is>
       </c>
       <c r="CS1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN4</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN4</t>
         </is>
       </c>
       <c r="CT1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN4</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN4</t>
         </is>
       </c>
       <c r="CU1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN5</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN5</t>
         </is>
       </c>
       <c r="CV1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN5</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN5</t>
         </is>
       </c>
       <c r="CW1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN5</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN5</t>
         </is>
       </c>
       <c r="CX1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN5</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN5</t>
         </is>
       </c>
       <c r="CY1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN5</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN5</t>
         </is>
       </c>
       <c r="CZ1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN6</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN6</t>
         </is>
       </c>
       <c r="DA1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN6</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN6</t>
         </is>
       </c>
       <c r="DB1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN6</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN6</t>
         </is>
       </c>
       <c r="DC1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN6</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN6</t>
         </is>
       </c>
       <c r="DD1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN6</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN6</t>
         </is>
       </c>
       <c r="DE1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN7</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN7</t>
         </is>
       </c>
       <c r="DF1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN7</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN7</t>
         </is>
       </c>
       <c r="DG1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN7</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN7</t>
         </is>
       </c>
       <c r="DH1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN7</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN7</t>
         </is>
       </c>
       <c r="DI1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN7</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN7</t>
         </is>
       </c>
       <c r="DJ1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN8</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN8</t>
         </is>
       </c>
       <c r="DK1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN8</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN8</t>
         </is>
       </c>
       <c r="DL1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN8</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN8</t>
         </is>
       </c>
       <c r="DM1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN8</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN8</t>
         </is>
       </c>
       <c r="DN1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN8</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN8</t>
         </is>
       </c>
       <c r="DO1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN9</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN9</t>
         </is>
       </c>
       <c r="DP1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN9</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN9</t>
         </is>
       </c>
       <c r="DQ1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN9</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN9</t>
         </is>
       </c>
       <c r="DR1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN9</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN9</t>
         </is>
       </c>
       <c r="DS1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN9</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN9</t>
         </is>
       </c>
       <c r="DT1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN10</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN10</t>
         </is>
       </c>
       <c r="DU1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN10</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN10</t>
         </is>
       </c>
       <c r="DV1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN10</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN10</t>
         </is>
       </c>
       <c r="DW1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN10</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN10</t>
         </is>
       </c>
       <c r="DX1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN10</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN10</t>
         </is>
       </c>
       <c r="DY1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN11</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN11</t>
         </is>
       </c>
       <c r="DZ1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN11</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN11</t>
         </is>
       </c>
       <c r="EA1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN11</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN11</t>
         </is>
       </c>
       <c r="EB1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN11</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN11</t>
         </is>
       </c>
       <c r="EC1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN11</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN11</t>
         </is>
       </c>
       <c r="ED1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN12</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN12</t>
         </is>
       </c>
       <c r="EE1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN12</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN12</t>
         </is>
       </c>
       <c r="EF1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN12</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN12</t>
         </is>
       </c>
       <c r="EG1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN12</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN12</t>
         </is>
       </c>
       <c r="EH1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN12</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN12</t>
         </is>
       </c>
       <c r="EI1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN13</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN13</t>
         </is>
       </c>
       <c r="EJ1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN13</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN13</t>
         </is>
       </c>
       <c r="EK1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN13</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN13</t>
         </is>
       </c>
       <c r="EL1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN13</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN13</t>
         </is>
       </c>
       <c r="EM1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN13</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN13</t>
         </is>
       </c>
       <c r="EN1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN14</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN14</t>
         </is>
       </c>
       <c r="EO1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN14</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN14</t>
         </is>
       </c>
       <c r="EP1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN14</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN14</t>
         </is>
       </c>
       <c r="EQ1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN14</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN14</t>
         </is>
       </c>
       <c r="ER1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN14</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN14</t>
         </is>
       </c>
       <c r="ES1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN15</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN15</t>
         </is>
       </c>
       <c r="ET1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN15</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN15</t>
         </is>
       </c>
       <c r="EU1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN15</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN15</t>
         </is>
       </c>
       <c r="EV1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN15</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN15</t>
         </is>
       </c>
       <c r="EW1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN15</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN15</t>
         </is>
       </c>
       <c r="EX1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN16</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN16</t>
         </is>
       </c>
       <c r="EY1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN16</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN16</t>
         </is>
       </c>
       <c r="EZ1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN16</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN16</t>
         </is>
       </c>
       <c r="FA1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN16</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN16</t>
         </is>
       </c>
       <c r="FB1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN16</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN16</t>
         </is>
       </c>
       <c r="FC1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN17</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN17</t>
         </is>
       </c>
       <c r="FD1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN17</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN17</t>
         </is>
       </c>
       <c r="FE1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN17</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN17</t>
         </is>
       </c>
       <c r="FF1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN17</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN17</t>
         </is>
       </c>
       <c r="FG1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN17</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN17</t>
         </is>
       </c>
       <c r="FH1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN18</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN18</t>
         </is>
       </c>
       <c r="FI1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN18</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN18</t>
         </is>
       </c>
       <c r="FJ1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN18</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN18</t>
         </is>
       </c>
       <c r="FK1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN18</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN18</t>
         </is>
       </c>
       <c r="FL1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN18</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN18</t>
         </is>
       </c>
       <c r="FM1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN19</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN19</t>
         </is>
       </c>
       <c r="FN1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN19</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN19</t>
         </is>
       </c>
       <c r="FO1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN19</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN19</t>
         </is>
       </c>
       <c r="FP1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN19</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN19</t>
         </is>
       </c>
       <c r="FQ1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN19</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN19</t>
         </is>
       </c>
       <c r="FR1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN20</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN20</t>
         </is>
       </c>
       <c r="FS1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN20</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN20</t>
         </is>
       </c>
       <c r="FT1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN20</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN20</t>
         </is>
       </c>
       <c r="FU1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN20</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN20</t>
         </is>
       </c>
       <c r="FV1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN20</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN20</t>
         </is>
       </c>
       <c r="FW1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN21</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN21</t>
         </is>
       </c>
       <c r="FX1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN21</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN21</t>
         </is>
       </c>
       <c r="FY1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN21</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN21</t>
         </is>
       </c>
       <c r="FZ1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN21</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN21</t>
         </is>
       </c>
       <c r="GA1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN21</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN21</t>
         </is>
       </c>
       <c r="GB1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN22</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN22</t>
         </is>
       </c>
       <c r="GC1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN22</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN22</t>
         </is>
       </c>
       <c r="GD1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN22</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN22</t>
         </is>
       </c>
       <c r="GE1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN22</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN22</t>
         </is>
       </c>
       <c r="GF1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN22</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN22</t>
         </is>
       </c>
       <c r="GG1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN23</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN23</t>
         </is>
       </c>
       <c r="GH1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN23</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN23</t>
         </is>
       </c>
       <c r="GI1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN23</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN23</t>
         </is>
       </c>
       <c r="GJ1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN23</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN23</t>
         </is>
       </c>
       <c r="GK1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN23</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN23</t>
         </is>
       </c>
       <c r="GL1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN24</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN24</t>
         </is>
       </c>
       <c r="GM1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN24</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN24</t>
         </is>
       </c>
       <c r="GN1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN24</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN24</t>
         </is>
       </c>
       <c r="GO1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN24</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN24</t>
         </is>
       </c>
       <c r="GP1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN24</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN24</t>
         </is>
       </c>
       <c r="GQ1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN25</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN25</t>
         </is>
       </c>
       <c r="GR1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN25</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN25</t>
         </is>
       </c>
       <c r="GS1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN25</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN25</t>
         </is>
       </c>
       <c r="GT1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN25</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN25</t>
         </is>
       </c>
       <c r="GU1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN25</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN25</t>
         </is>
       </c>
       <c r="GV1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN26</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN26</t>
         </is>
       </c>
       <c r="GW1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN26</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN26</t>
         </is>
       </c>
       <c r="GX1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN26</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN26</t>
         </is>
       </c>
       <c r="GY1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN26</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN26</t>
         </is>
       </c>
       <c r="GZ1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN26</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN26</t>
         </is>
       </c>
       <c r="HA1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN27</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN27</t>
         </is>
       </c>
       <c r="HB1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN27</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN27</t>
         </is>
       </c>
       <c r="HC1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN27</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN27</t>
         </is>
       </c>
       <c r="HD1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN27</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN27</t>
         </is>
       </c>
       <c r="HE1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN27</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN27</t>
         </is>
       </c>
       <c r="HF1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN28</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN28</t>
         </is>
       </c>
       <c r="HG1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN28</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN28</t>
         </is>
       </c>
       <c r="HH1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN28</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN28</t>
         </is>
       </c>
       <c r="HI1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN28</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN28</t>
         </is>
       </c>
       <c r="HJ1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN28</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN28</t>
         </is>
       </c>
       <c r="HK1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN29</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN29</t>
         </is>
       </c>
       <c r="HL1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN29</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN29</t>
         </is>
       </c>
       <c r="HM1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN29</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN29</t>
         </is>
       </c>
       <c r="HN1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN29</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN29</t>
         </is>
       </c>
       <c r="HO1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN29</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN29</t>
         </is>
       </c>
       <c r="HP1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN30</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN30</t>
         </is>
       </c>
       <c r="HQ1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN30</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN30</t>
         </is>
       </c>
       <c r="HR1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN30</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN30</t>
         </is>
       </c>
       <c r="HS1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN30</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN30</t>
         </is>
       </c>
       <c r="HT1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN30</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN30</t>
         </is>
       </c>
       <c r="HU1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN31</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN31</t>
         </is>
       </c>
       <c r="HV1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN31</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN31</t>
         </is>
       </c>
       <c r="HW1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN31</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN31</t>
         </is>
       </c>
       <c r="HX1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN31</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN31</t>
         </is>
       </c>
       <c r="HY1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN31</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN31</t>
         </is>
       </c>
       <c r="HZ1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN32</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN32</t>
         </is>
       </c>
       <c r="IA1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN32</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN32</t>
         </is>
       </c>
       <c r="IB1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN32</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN32</t>
         </is>
       </c>
       <c r="IC1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN32</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN32</t>
         </is>
       </c>
       <c r="ID1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN32</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN32</t>
         </is>
       </c>
       <c r="IE1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN33</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN33</t>
         </is>
       </c>
       <c r="IF1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN33</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN33</t>
         </is>
       </c>
       <c r="IG1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN33</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN33</t>
         </is>
       </c>
       <c r="IH1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN33</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN33</t>
         </is>
       </c>
       <c r="II1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN33</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN33</t>
         </is>
       </c>
       <c r="IJ1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN34</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN34</t>
         </is>
       </c>
       <c r="IK1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN34</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN34</t>
         </is>
       </c>
       <c r="IL1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN34</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN34</t>
         </is>
       </c>
       <c r="IM1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN34</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN34</t>
         </is>
       </c>
       <c r="IN1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN34</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN34</t>
         </is>
       </c>
       <c r="IO1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN35</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN35</t>
         </is>
       </c>
       <c r="IP1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN35</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN35</t>
         </is>
       </c>
       <c r="IQ1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN35</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN35</t>
         </is>
       </c>
       <c r="IR1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN35</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN35</t>
         </is>
       </c>
       <c r="IS1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN35</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN35</t>
         </is>
       </c>
       <c r="IT1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN36</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN36</t>
         </is>
       </c>
       <c r="IU1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN36</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN36</t>
         </is>
       </c>
       <c r="IV1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN36</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN36</t>
         </is>
       </c>
       <c r="IW1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN36</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN36</t>
         </is>
       </c>
       <c r="IX1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN36</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN36</t>
         </is>
       </c>
       <c r="IY1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN37</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN37</t>
         </is>
       </c>
       <c r="IZ1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN37</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN37</t>
         </is>
       </c>
       <c r="JA1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN37</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN37</t>
         </is>
       </c>
       <c r="JB1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN37</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN37</t>
         </is>
       </c>
       <c r="JC1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN37</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN37</t>
         </is>
       </c>
       <c r="JD1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN38</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN38</t>
         </is>
       </c>
       <c r="JE1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN38</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN38</t>
         </is>
       </c>
       <c r="JF1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN38</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN38</t>
         </is>
       </c>
       <c r="JG1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN38</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN38</t>
         </is>
       </c>
       <c r="JH1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN38</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN38</t>
         </is>
       </c>
       <c r="JI1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN39</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN39</t>
         </is>
       </c>
       <c r="JJ1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN39</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN39</t>
         </is>
       </c>
       <c r="JK1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN39</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN39</t>
         </is>
       </c>
       <c r="JL1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN39</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN39</t>
         </is>
       </c>
       <c r="JM1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN39</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN39</t>
         </is>
       </c>
       <c r="JN1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN40</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN40</t>
         </is>
       </c>
       <c r="JO1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN40</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN40</t>
         </is>
       </c>
       <c r="JP1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN40</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN40</t>
         </is>
       </c>
       <c r="JQ1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN40</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN40</t>
         </is>
       </c>
       <c r="JR1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN40</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN40</t>
         </is>
       </c>
       <c r="JS1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MEAN)//INTENSITY//RINGS_EDGE_PROFILE_BIN41</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN41</t>
         </is>
       </c>
       <c r="JT1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MIN)//INTENSITY//RINGS_EDGE_PROFILE_BIN41</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN41</t>
         </is>
       </c>
       <c r="JU1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_MAX)//INTENSITY//RINGS_EDGE_PROFILE_BIN41</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN41</t>
         </is>
       </c>
       <c r="JV1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_STD)//INTENSITY//RINGS_EDGE_PROFILE_BIN41</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN41</t>
         </is>
       </c>
       <c r="JW1" t="inlineStr">
         <is>
-          <t>RING_(OBJ_SUM)//INTENSITY//RINGS_EDGE_PROFILE_BIN41</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN41</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>E:\Stephen\Java Projects\ModularImageAnalysis\src\test\resources\images\BinarySphere3D_8bit.tif</t>
+          <t>C:\Users\steph\Documents\Java Projects\ModularImageAnalysis\src\test\resources\images\BinarySphere3D_8bit.tif</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -2548,23 +2548,23 @@
       <c r="CE2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="CF2" t="e">
-        <v>#NUM!</v>
+      <c r="CF2" t="n">
+        <v>0.0</v>
       </c>
       <c r="CI2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="CJ2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="CK2" t="e">
-        <v>#NUM!</v>
+      <c r="CJ2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="CK2" t="n">
+        <v>0.0</v>
       </c>
       <c r="CN2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="CO2" t="e">
-        <v>#NUM!</v>
+      <c r="CO2" t="n">
+        <v>0.0</v>
       </c>
       <c r="CP2" t="n">
         <v>0.0</v>
@@ -2719,14 +2719,14 @@
       <c r="FV2" t="n">
         <v>0.0</v>
       </c>
-      <c r="FW2" t="n">
-        <v>0.0</v>
+      <c r="FW2" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="FZ2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="GA2" t="n">
-        <v>0.0</v>
+      <c r="GA2" t="e">
+        <v>#NUM!</v>
       </c>
       <c r="GB2" t="n">
         <v>0.0</v>
@@ -2809,23 +2809,23 @@
       <c r="HT2" t="n">
         <v>0.0</v>
       </c>
-      <c r="HU2" t="e">
-        <v>#NUM!</v>
+      <c r="HU2" t="n">
+        <v>25.31476997578695</v>
       </c>
       <c r="HX2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="HY2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="HZ2" t="e">
-        <v>#NUM!</v>
+      <c r="HY2" t="n">
+        <v>25.31476997578695</v>
+      </c>
+      <c r="HZ2" t="n">
+        <v>5.710808179162615</v>
       </c>
       <c r="IC2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="ID2" t="e">
-        <v>#NUM!</v>
+      <c r="ID2" t="n">
+        <v>5.710808179162615</v>
       </c>
       <c r="IE2" t="n">
         <v>0.0</v>
@@ -2900,13 +2900,13 @@
         <v>0.0</v>
       </c>
       <c r="JS2" t="n">
-        <v>2.090633423180601</v>
+        <v>0.0</v>
       </c>
       <c r="JV2" t="e">
         <v>#NUM!</v>
       </c>
       <c r="JW2" t="n">
-        <v>2.090633423180601</v>
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
@@ -2945,282 +2945,282 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_MEAN</t>
+          <t>INTENSITY//Shell_MEAN</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_MIN</t>
+          <t>INTENSITY//Shell_MIN</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_MAX</t>
+          <t>INTENSITY//Shell_MAX</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_STDEV</t>
+          <t>INTENSITY//Shell_STDEV</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_SUM</t>
+          <t>INTENSITY//Shell_SUM</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_X_CENTRE_MEAN (PX)</t>
+          <t>INTENSITY//Shell_X_CENTRE_MEAN (PX)</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_X_CENTRE_STDEV (PX)</t>
+          <t>INTENSITY//Shell_X_CENTRE_STDEV (PX)</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_Y_CENTRE_MEAN (PX)</t>
+          <t>INTENSITY//Shell_Y_CENTRE_MEAN (PX)</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_Y_CENTRE_STDEV (PX)</t>
+          <t>INTENSITY//Shell_Y_CENTRE_STDEV (PX)</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_Z_CENTRE_MEAN (SLICE)</t>
+          <t>INTENSITY//Shell_Z_CENTRE_MEAN (SLICE)</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_Z_CENTRE_STDEV (SLICE)</t>
+          <t>INTENSITY//Shell_Z_CENTRE_STDEV (SLICE)</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_MEAN_EDGE_DISTANCE (PX)</t>
+          <t>INTENSITY//Shell_MEAN_EDGE_DISTANCE (PX)</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_MEAN_EDGE_DISTANCE (CAL)</t>
+          <t>INTENSITY//Shell_MEAN_EDGE_DISTANCE (CAL)</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_STD_EDGE_DISTANCE (PX)</t>
+          <t>INTENSITY//Shell_STD_EDGE_DISTANCE (PX)</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_STD_EDGE_DISTANCE (CAL)</t>
+          <t>INTENSITY//Shell_STD_EDGE_DISTANCE (CAL)</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN1</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN1</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN2</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN2</t>
         </is>
       </c>
       <c r="V1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN3</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN3</t>
         </is>
       </c>
       <c r="W1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN4</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN4</t>
         </is>
       </c>
       <c r="X1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN5</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN5</t>
         </is>
       </c>
       <c r="Y1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN6</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN6</t>
         </is>
       </c>
       <c r="Z1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN7</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN7</t>
         </is>
       </c>
       <c r="AA1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN8</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN8</t>
         </is>
       </c>
       <c r="AB1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN9</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN9</t>
         </is>
       </c>
       <c r="AC1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN10</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN10</t>
         </is>
       </c>
       <c r="AD1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN11</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN11</t>
         </is>
       </c>
       <c r="AE1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN12</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN12</t>
         </is>
       </c>
       <c r="AF1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN13</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN13</t>
         </is>
       </c>
       <c r="AG1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN14</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN14</t>
         </is>
       </c>
       <c r="AH1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN15</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN15</t>
         </is>
       </c>
       <c r="AI1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN16</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN16</t>
         </is>
       </c>
       <c r="AJ1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN17</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN17</t>
         </is>
       </c>
       <c r="AK1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN18</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN18</t>
         </is>
       </c>
       <c r="AL1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN19</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN19</t>
         </is>
       </c>
       <c r="AM1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN20</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN20</t>
         </is>
       </c>
       <c r="AN1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN21</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN21</t>
         </is>
       </c>
       <c r="AO1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN22</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN22</t>
         </is>
       </c>
       <c r="AP1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN23</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN23</t>
         </is>
       </c>
       <c r="AQ1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN24</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN24</t>
         </is>
       </c>
       <c r="AR1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN25</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN25</t>
         </is>
       </c>
       <c r="AS1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN26</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN26</t>
         </is>
       </c>
       <c r="AT1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN27</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN27</t>
         </is>
       </c>
       <c r="AU1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN28</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN28</t>
         </is>
       </c>
       <c r="AV1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN29</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN29</t>
         </is>
       </c>
       <c r="AW1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN30</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN30</t>
         </is>
       </c>
       <c r="AX1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN31</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN31</t>
         </is>
       </c>
       <c r="AY1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN32</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN32</t>
         </is>
       </c>
       <c r="AZ1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN33</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN33</t>
         </is>
       </c>
       <c r="BA1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN34</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN34</t>
         </is>
       </c>
       <c r="BB1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN35</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN35</t>
         </is>
       </c>
       <c r="BC1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN36</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN36</t>
         </is>
       </c>
       <c r="BD1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN37</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN37</t>
         </is>
       </c>
       <c r="BE1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN38</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN38</t>
         </is>
       </c>
       <c r="BF1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN39</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN39</t>
         </is>
       </c>
       <c r="BG1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN40</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN40</t>
         </is>
       </c>
       <c r="BH1" t="inlineStr">
         <is>
-          <t>INTENSITY//Rings_EDGE_PROFILE_BIN41</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN41</t>
         </is>
       </c>
     </row>
@@ -3230,7 +3230,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>E:\Stephen\Java Projects\ModularImageAnalysis\src\test\resources\images\BinarySphere3D_8bit.tif</t>
+          <t>C:\Users\steph\Documents\Java Projects\ModularImageAnalysis\src\test\resources\images\BinarySphere3D_8bit.tif</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -3303,70 +3303,68 @@
           <t/>
         </is>
       </c>
-      <c r="U2" t="inlineStr">
+      <c r="U2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="V2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="W2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="X2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Y2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AA2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AB2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AC2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AF2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AG2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AK2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AL2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AN2" t="inlineStr">
         <is>
           <t/>
         </is>
       </c>
-      <c r="V2" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="W2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="X2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Y2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="Z2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AA2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AB2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AC2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AD2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AE2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AF2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AG2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AH2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AI2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AJ2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AK2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AL2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AM2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AN2" t="n">
-        <v>0.0</v>
-      </c>
       <c r="AO2" t="n">
         <v>0.0</v>
       </c>
@@ -3394,15 +3392,11 @@
       <c r="AW2" t="n">
         <v>0.0</v>
       </c>
-      <c r="AX2" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="AY2" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+      <c r="AX2" t="n">
+        <v>25.31476997578695</v>
+      </c>
+      <c r="AY2" t="n">
+        <v>5.710808179162615</v>
       </c>
       <c r="AZ2" t="n">
         <v>0.0</v>
@@ -3429,7 +3423,7 @@
         <v>0.0</v>
       </c>
       <c r="BH2" t="n">
-        <v>2.090633423180601</v>
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor edits to intensity profile measurements
Updated MeasureObjectIntensity to remove missing measurements at zero distance from object edge.

Corrected errors with calibrated distance intensity profile bins.
</commit_message>
<xml_diff>
--- a/src/test/resources/images/BinarySphere3D_8bit1.xlsx
+++ b/src/test/resources/images/BinarySphere3D_8bit1.xlsx
@@ -390,7 +390,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>C:\Users\steph\Documents\Java Projects\ModularImageAnalysis\src\test\resources\images\MeasureObjectIntensity\BinarySphere3D_10pxOutsideShell_8bit.tif</t>
+          <t>C:\Users\steph\Documents\Java Projects\ModularImageAnalysis\src\test\resources\images\MeasureObjectIntensity\BinarySphere3D_1pxInside10pxOutsideShell_8bit.tif</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -696,7 +696,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>false</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
@@ -747,7 +747,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>false</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
@@ -764,7 +764,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>false</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -781,7 +781,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>false</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
@@ -798,7 +798,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>false</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
@@ -815,7 +815,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>false</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
@@ -832,7 +832,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>false</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
@@ -849,7 +849,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>false</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
@@ -861,12 +861,12 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Edge distance mode</t>
+          <t>Measure intensity profile from edge</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Inside and outside</t>
+          <t>true</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
@@ -878,12 +878,12 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Measure intensity profile from edge</t>
+          <t>Minimum distance</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>true</t>
+          <t>-15.0</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
@@ -895,12 +895,12 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Minimum distance</t>
+          <t>Maximum distance</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>-20.0</t>
+          <t>15.0</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
@@ -912,12 +912,12 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Maximum distance</t>
+          <t>Calibrated distances</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>20.0</t>
+          <t>false</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
@@ -929,32 +929,15 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Calibrated distances</t>
+          <t>Number of measurements</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>false</t>
+          <t>41</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
-        <is>
-          <t>MeasureObjectIntensity</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>Number of measurements</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>41</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
         <is>
           <t>MeasureObjectIntensity</t>
         </is>
@@ -991,1402 +974,1027 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_MEAN</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN01_(-15.00PX)</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_MEAN</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN01_(-15.00PX)</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_MEAN</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN01_(-15.00PX)</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_MEAN</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN01_(-15.00PX)</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_MEAN</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN01_(-15.00PX)</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_MIN</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN02_(-14.25PX)</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_MIN</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN02_(-14.25PX)</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_MIN</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN02_(-14.25PX)</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_MIN</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN02_(-14.25PX)</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_MIN</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN02_(-14.25PX)</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_MAX</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN03_(-13.50PX)</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_MAX</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN03_(-13.50PX)</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_MAX</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN03_(-13.50PX)</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_MAX</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN03_(-13.50PX)</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_MAX</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN03_(-13.50PX)</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_STDEV</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN04_(-12.75PX)</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_STDEV</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN04_(-12.75PX)</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_STDEV</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN04_(-12.75PX)</t>
         </is>
       </c>
       <c r="V1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_STDEV</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN04_(-12.75PX)</t>
         </is>
       </c>
       <c r="W1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_STDEV</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN04_(-12.75PX)</t>
         </is>
       </c>
       <c r="X1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_SUM</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN05_(-12.00PX)</t>
         </is>
       </c>
       <c r="Y1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_SUM</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN05_(-12.00PX)</t>
         </is>
       </c>
       <c r="Z1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_SUM</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN05_(-12.00PX)</t>
         </is>
       </c>
       <c r="AA1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_SUM</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN05_(-12.00PX)</t>
         </is>
       </c>
       <c r="AB1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_SUM</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN05_(-12.00PX)</t>
         </is>
       </c>
       <c r="AC1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_X_CENTRE_MEAN_(PX)</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN06_(-11.25PX)</t>
         </is>
       </c>
       <c r="AD1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_X_CENTRE_MEAN_(PX)</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN06_(-11.25PX)</t>
         </is>
       </c>
       <c r="AE1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_X_CENTRE_MEAN_(PX)</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN06_(-11.25PX)</t>
         </is>
       </c>
       <c r="AF1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_X_CENTRE_MEAN_(PX)</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN06_(-11.25PX)</t>
         </is>
       </c>
       <c r="AG1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_X_CENTRE_MEAN_(PX)</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN06_(-11.25PX)</t>
         </is>
       </c>
       <c r="AH1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_X_CENTRE_STDEV_(PX)</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN07_(-10.50PX)</t>
         </is>
       </c>
       <c r="AI1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_X_CENTRE_STDEV_(PX)</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN07_(-10.50PX)</t>
         </is>
       </c>
       <c r="AJ1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_X_CENTRE_STDEV_(PX)</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN07_(-10.50PX)</t>
         </is>
       </c>
       <c r="AK1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_X_CENTRE_STDEV_(PX)</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN07_(-10.50PX)</t>
         </is>
       </c>
       <c r="AL1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_X_CENTRE_STDEV_(PX)</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN07_(-10.50PX)</t>
         </is>
       </c>
       <c r="AM1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_Y_CENTRE_MEAN_(PX)</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN08_(-9.75PX)</t>
         </is>
       </c>
       <c r="AN1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_Y_CENTRE_MEAN_(PX)</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN08_(-9.75PX)</t>
         </is>
       </c>
       <c r="AO1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_Y_CENTRE_MEAN_(PX)</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN08_(-9.75PX)</t>
         </is>
       </c>
       <c r="AP1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_Y_CENTRE_MEAN_(PX)</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN08_(-9.75PX)</t>
         </is>
       </c>
       <c r="AQ1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_Y_CENTRE_MEAN_(PX)</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN08_(-9.75PX)</t>
         </is>
       </c>
       <c r="AR1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_Y_CENTRE_STDEV_(PX)</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN09_(-9.00PX)</t>
         </is>
       </c>
       <c r="AS1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_Y_CENTRE_STDEV_(PX)</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN09_(-9.00PX)</t>
         </is>
       </c>
       <c r="AT1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_Y_CENTRE_STDEV_(PX)</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN09_(-9.00PX)</t>
         </is>
       </c>
       <c r="AU1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_Y_CENTRE_STDEV_(PX)</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN09_(-9.00PX)</t>
         </is>
       </c>
       <c r="AV1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_Y_CENTRE_STDEV_(PX)</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN09_(-9.00PX)</t>
         </is>
       </c>
       <c r="AW1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_Z_CENTRE_MEAN_(SLICE)</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN10_(-8.25PX)</t>
         </is>
       </c>
       <c r="AX1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_Z_CENTRE_MEAN_(SLICE)</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN10_(-8.25PX)</t>
         </is>
       </c>
       <c r="AY1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_Z_CENTRE_MEAN_(SLICE)</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN10_(-8.25PX)</t>
         </is>
       </c>
       <c r="AZ1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_Z_CENTRE_MEAN_(SLICE)</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN10_(-8.25PX)</t>
         </is>
       </c>
       <c r="BA1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_Z_CENTRE_MEAN_(SLICE)</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN10_(-8.25PX)</t>
         </is>
       </c>
       <c r="BB1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_Z_CENTRE_STDEV_(SLICE)</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN11_(-7.50PX)</t>
         </is>
       </c>
       <c r="BC1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_Z_CENTRE_STDEV_(SLICE)</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN11_(-7.50PX)</t>
         </is>
       </c>
       <c r="BD1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_Z_CENTRE_STDEV_(SLICE)</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN11_(-7.50PX)</t>
         </is>
       </c>
       <c r="BE1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_Z_CENTRE_STDEV_(SLICE)</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN11_(-7.50PX)</t>
         </is>
       </c>
       <c r="BF1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_Z_CENTRE_STDEV_(SLICE)</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN11_(-7.50PX)</t>
         </is>
       </c>
       <c r="BG1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_MEAN_EDGE_DISTANCE_(PX)</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN12_(-6.75PX)</t>
         </is>
       </c>
       <c r="BH1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_MEAN_EDGE_DISTANCE_(PX)</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN12_(-6.75PX)</t>
         </is>
       </c>
       <c r="BI1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_MEAN_EDGE_DISTANCE_(PX)</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN12_(-6.75PX)</t>
         </is>
       </c>
       <c r="BJ1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_MEAN_EDGE_DISTANCE_(PX)</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN12_(-6.75PX)</t>
         </is>
       </c>
       <c r="BK1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_MEAN_EDGE_DISTANCE_(PX)</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN12_(-6.75PX)</t>
         </is>
       </c>
       <c r="BL1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_MEAN_EDGE_DISTANCE_(CAL)</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN13_(-6.00PX)</t>
         </is>
       </c>
       <c r="BM1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_MEAN_EDGE_DISTANCE_(CAL)</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN13_(-6.00PX)</t>
         </is>
       </c>
       <c r="BN1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_MEAN_EDGE_DISTANCE_(CAL)</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN13_(-6.00PX)</t>
         </is>
       </c>
       <c r="BO1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_MEAN_EDGE_DISTANCE_(CAL)</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN13_(-6.00PX)</t>
         </is>
       </c>
       <c r="BP1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_MEAN_EDGE_DISTANCE_(CAL)</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN13_(-6.00PX)</t>
         </is>
       </c>
       <c r="BQ1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_STD_EDGE_DISTANCE_(PX)</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN14_(-5.25PX)</t>
         </is>
       </c>
       <c r="BR1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_STD_EDGE_DISTANCE_(PX)</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN14_(-5.25PX)</t>
         </is>
       </c>
       <c r="BS1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_STD_EDGE_DISTANCE_(PX)</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN14_(-5.25PX)</t>
         </is>
       </c>
       <c r="BT1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_STD_EDGE_DISTANCE_(PX)</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN14_(-5.25PX)</t>
         </is>
       </c>
       <c r="BU1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_STD_EDGE_DISTANCE_(PX)</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN14_(-5.25PX)</t>
         </is>
       </c>
       <c r="BV1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_STD_EDGE_DISTANCE_(CAL)</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN15_(-4.50PX)</t>
         </is>
       </c>
       <c r="BW1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_STD_EDGE_DISTANCE_(CAL)</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN15_(-4.50PX)</t>
         </is>
       </c>
       <c r="BX1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_STD_EDGE_DISTANCE_(CAL)</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN15_(-4.50PX)</t>
         </is>
       </c>
       <c r="BY1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_STD_EDGE_DISTANCE_(CAL)</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN15_(-4.50PX)</t>
         </is>
       </c>
       <c r="BZ1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_STD_EDGE_DISTANCE_(CAL)</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN15_(-4.50PX)</t>
         </is>
       </c>
       <c r="CA1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN1</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN16_(-3.75PX)</t>
         </is>
       </c>
       <c r="CB1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN1</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN16_(-3.75PX)</t>
         </is>
       </c>
       <c r="CC1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN1</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN16_(-3.75PX)</t>
         </is>
       </c>
       <c r="CD1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN1</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN16_(-3.75PX)</t>
         </is>
       </c>
       <c r="CE1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN1</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN16_(-3.75PX)</t>
         </is>
       </c>
       <c r="CF1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN2</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN17_(-3.00PX)</t>
         </is>
       </c>
       <c r="CG1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN2</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN17_(-3.00PX)</t>
         </is>
       </c>
       <c r="CH1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN2</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN17_(-3.00PX)</t>
         </is>
       </c>
       <c r="CI1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN2</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN17_(-3.00PX)</t>
         </is>
       </c>
       <c r="CJ1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN2</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN17_(-3.00PX)</t>
         </is>
       </c>
       <c r="CK1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN3</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN18_(-2.25PX)</t>
         </is>
       </c>
       <c r="CL1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN3</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN18_(-2.25PX)</t>
         </is>
       </c>
       <c r="CM1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN3</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN18_(-2.25PX)</t>
         </is>
       </c>
       <c r="CN1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN3</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN18_(-2.25PX)</t>
         </is>
       </c>
       <c r="CO1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN3</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN18_(-2.25PX)</t>
         </is>
       </c>
       <c r="CP1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN4</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN19_(-1.50PX)</t>
         </is>
       </c>
       <c r="CQ1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN4</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN19_(-1.50PX)</t>
         </is>
       </c>
       <c r="CR1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN4</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN19_(-1.50PX)</t>
         </is>
       </c>
       <c r="CS1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN4</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN19_(-1.50PX)</t>
         </is>
       </c>
       <c r="CT1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN4</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN19_(-1.50PX)</t>
         </is>
       </c>
       <c r="CU1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN5</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN20_(-.75PX)</t>
         </is>
       </c>
       <c r="CV1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN5</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN20_(-.75PX)</t>
         </is>
       </c>
       <c r="CW1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN5</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN20_(-.75PX)</t>
         </is>
       </c>
       <c r="CX1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN5</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN20_(-.75PX)</t>
         </is>
       </c>
       <c r="CY1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN5</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN20_(-.75PX)</t>
         </is>
       </c>
       <c r="CZ1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN6</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN21_(.00PX)</t>
         </is>
       </c>
       <c r="DA1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN6</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN21_(.00PX)</t>
         </is>
       </c>
       <c r="DB1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN6</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN21_(.00PX)</t>
         </is>
       </c>
       <c r="DC1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN6</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN21_(.00PX)</t>
         </is>
       </c>
       <c r="DD1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN6</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN21_(.00PX)</t>
         </is>
       </c>
       <c r="DE1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN7</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN22_(.75PX)</t>
         </is>
       </c>
       <c r="DF1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN7</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN22_(.75PX)</t>
         </is>
       </c>
       <c r="DG1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN7</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN22_(.75PX)</t>
         </is>
       </c>
       <c r="DH1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN7</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN22_(.75PX)</t>
         </is>
       </c>
       <c r="DI1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN7</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN22_(.75PX)</t>
         </is>
       </c>
       <c r="DJ1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN8</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN23_(1.50PX)</t>
         </is>
       </c>
       <c r="DK1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN8</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN23_(1.50PX)</t>
         </is>
       </c>
       <c r="DL1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN8</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN23_(1.50PX)</t>
         </is>
       </c>
       <c r="DM1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN8</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN23_(1.50PX)</t>
         </is>
       </c>
       <c r="DN1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN8</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN23_(1.50PX)</t>
         </is>
       </c>
       <c r="DO1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN9</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN24_(2.25PX)</t>
         </is>
       </c>
       <c r="DP1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN9</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN24_(2.25PX)</t>
         </is>
       </c>
       <c r="DQ1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN9</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN24_(2.25PX)</t>
         </is>
       </c>
       <c r="DR1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN9</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN24_(2.25PX)</t>
         </is>
       </c>
       <c r="DS1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN9</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN24_(2.25PX)</t>
         </is>
       </c>
       <c r="DT1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN10</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN25_(3.00PX)</t>
         </is>
       </c>
       <c r="DU1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN10</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN25_(3.00PX)</t>
         </is>
       </c>
       <c r="DV1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN10</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN25_(3.00PX)</t>
         </is>
       </c>
       <c r="DW1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN10</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN25_(3.00PX)</t>
         </is>
       </c>
       <c r="DX1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN10</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN25_(3.00PX)</t>
         </is>
       </c>
       <c r="DY1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN11</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN26_(3.75PX)</t>
         </is>
       </c>
       <c r="DZ1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN11</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN26_(3.75PX)</t>
         </is>
       </c>
       <c r="EA1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN11</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN26_(3.75PX)</t>
         </is>
       </c>
       <c r="EB1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN11</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN26_(3.75PX)</t>
         </is>
       </c>
       <c r="EC1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN11</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN26_(3.75PX)</t>
         </is>
       </c>
       <c r="ED1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN12</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN27_(4.50PX)</t>
         </is>
       </c>
       <c r="EE1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN12</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN27_(4.50PX)</t>
         </is>
       </c>
       <c r="EF1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN12</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN27_(4.50PX)</t>
         </is>
       </c>
       <c r="EG1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN12</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN27_(4.50PX)</t>
         </is>
       </c>
       <c r="EH1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN12</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN27_(4.50PX)</t>
         </is>
       </c>
       <c r="EI1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN13</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN28_(5.25PX)</t>
         </is>
       </c>
       <c r="EJ1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN13</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN28_(5.25PX)</t>
         </is>
       </c>
       <c r="EK1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN13</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN28_(5.25PX)</t>
         </is>
       </c>
       <c r="EL1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN13</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN28_(5.25PX)</t>
         </is>
       </c>
       <c r="EM1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN13</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN28_(5.25PX)</t>
         </is>
       </c>
       <c r="EN1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN14</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN29_(6.00PX)</t>
         </is>
       </c>
       <c r="EO1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN14</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN29_(6.00PX)</t>
         </is>
       </c>
       <c r="EP1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN14</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN29_(6.00PX)</t>
         </is>
       </c>
       <c r="EQ1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN14</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN29_(6.00PX)</t>
         </is>
       </c>
       <c r="ER1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN14</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN29_(6.00PX)</t>
         </is>
       </c>
       <c r="ES1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN15</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN30_(6.75PX)</t>
         </is>
       </c>
       <c r="ET1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN15</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN30_(6.75PX)</t>
         </is>
       </c>
       <c r="EU1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN15</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN30_(6.75PX)</t>
         </is>
       </c>
       <c r="EV1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN15</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN30_(6.75PX)</t>
         </is>
       </c>
       <c r="EW1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN15</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN30_(6.75PX)</t>
         </is>
       </c>
       <c r="EX1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN16</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN31_(7.50PX)</t>
         </is>
       </c>
       <c r="EY1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN16</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN31_(7.50PX)</t>
         </is>
       </c>
       <c r="EZ1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN16</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN31_(7.50PX)</t>
         </is>
       </c>
       <c r="FA1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN16</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN31_(7.50PX)</t>
         </is>
       </c>
       <c r="FB1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN16</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN31_(7.50PX)</t>
         </is>
       </c>
       <c r="FC1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN17</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN32_(8.25PX)</t>
         </is>
       </c>
       <c r="FD1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN17</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN32_(8.25PX)</t>
         </is>
       </c>
       <c r="FE1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN17</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN32_(8.25PX)</t>
         </is>
       </c>
       <c r="FF1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN17</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN32_(8.25PX)</t>
         </is>
       </c>
       <c r="FG1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN17</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN32_(8.25PX)</t>
         </is>
       </c>
       <c r="FH1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN18</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN33_(9.00PX)</t>
         </is>
       </c>
       <c r="FI1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN18</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN33_(9.00PX)</t>
         </is>
       </c>
       <c r="FJ1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN18</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN33_(9.00PX)</t>
         </is>
       </c>
       <c r="FK1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN18</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN33_(9.00PX)</t>
         </is>
       </c>
       <c r="FL1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN18</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN33_(9.00PX)</t>
         </is>
       </c>
       <c r="FM1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN19</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN34_(9.75PX)</t>
         </is>
       </c>
       <c r="FN1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN19</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN34_(9.75PX)</t>
         </is>
       </c>
       <c r="FO1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN19</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN34_(9.75PX)</t>
         </is>
       </c>
       <c r="FP1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN19</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN34_(9.75PX)</t>
         </is>
       </c>
       <c r="FQ1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN19</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN34_(9.75PX)</t>
         </is>
       </c>
       <c r="FR1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN20</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN35_(10.50PX)</t>
         </is>
       </c>
       <c r="FS1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN20</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN35_(10.50PX)</t>
         </is>
       </c>
       <c r="FT1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN20</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN35_(10.50PX)</t>
         </is>
       </c>
       <c r="FU1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN20</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN35_(10.50PX)</t>
         </is>
       </c>
       <c r="FV1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN20</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN35_(10.50PX)</t>
         </is>
       </c>
       <c r="FW1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN21</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN36_(11.25PX)</t>
         </is>
       </c>
       <c r="FX1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN21</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN36_(11.25PX)</t>
         </is>
       </c>
       <c r="FY1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN21</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN36_(11.25PX)</t>
         </is>
       </c>
       <c r="FZ1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN21</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN36_(11.25PX)</t>
         </is>
       </c>
       <c r="GA1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN21</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN36_(11.25PX)</t>
         </is>
       </c>
       <c r="GB1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN22</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN37_(12.00PX)</t>
         </is>
       </c>
       <c r="GC1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN22</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN37_(12.00PX)</t>
         </is>
       </c>
       <c r="GD1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN22</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN37_(12.00PX)</t>
         </is>
       </c>
       <c r="GE1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN22</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN37_(12.00PX)</t>
         </is>
       </c>
       <c r="GF1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN22</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN37_(12.00PX)</t>
         </is>
       </c>
       <c r="GG1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN23</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN38_(12.75PX)</t>
         </is>
       </c>
       <c r="GH1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN23</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN38_(12.75PX)</t>
         </is>
       </c>
       <c r="GI1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN23</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN38_(12.75PX)</t>
         </is>
       </c>
       <c r="GJ1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN23</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN38_(12.75PX)</t>
         </is>
       </c>
       <c r="GK1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN23</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN38_(12.75PX)</t>
         </is>
       </c>
       <c r="GL1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN24</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN39_(13.50PX)</t>
         </is>
       </c>
       <c r="GM1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN24</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN39_(13.50PX)</t>
         </is>
       </c>
       <c r="GN1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN24</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN39_(13.50PX)</t>
         </is>
       </c>
       <c r="GO1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN24</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN39_(13.50PX)</t>
         </is>
       </c>
       <c r="GP1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN24</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN39_(13.50PX)</t>
         </is>
       </c>
       <c r="GQ1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN25</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN40_(14.25PX)</t>
         </is>
       </c>
       <c r="GR1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN25</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN40_(14.25PX)</t>
         </is>
       </c>
       <c r="GS1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN25</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN40_(14.25PX)</t>
         </is>
       </c>
       <c r="GT1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN25</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN40_(14.25PX)</t>
         </is>
       </c>
       <c r="GU1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN25</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN40_(14.25PX)</t>
         </is>
       </c>
       <c r="GV1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN26</t>
+          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN41_(15.00PX)</t>
         </is>
       </c>
       <c r="GW1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN26</t>
+          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN41_(15.00PX)</t>
         </is>
       </c>
       <c r="GX1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN26</t>
+          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN41_(15.00PX)</t>
         </is>
       </c>
       <c r="GY1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN26</t>
+          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN41_(15.00PX)</t>
         </is>
       </c>
       <c r="GZ1" t="inlineStr">
         <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN26</t>
-        </is>
-      </c>
-      <c r="HA1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN27</t>
-        </is>
-      </c>
-      <c r="HB1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN27</t>
-        </is>
-      </c>
-      <c r="HC1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN27</t>
-        </is>
-      </c>
-      <c r="HD1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN27</t>
-        </is>
-      </c>
-      <c r="HE1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN27</t>
-        </is>
-      </c>
-      <c r="HF1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN28</t>
-        </is>
-      </c>
-      <c r="HG1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN28</t>
-        </is>
-      </c>
-      <c r="HH1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN28</t>
-        </is>
-      </c>
-      <c r="HI1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN28</t>
-        </is>
-      </c>
-      <c r="HJ1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN28</t>
-        </is>
-      </c>
-      <c r="HK1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN29</t>
-        </is>
-      </c>
-      <c r="HL1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN29</t>
-        </is>
-      </c>
-      <c r="HM1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN29</t>
-        </is>
-      </c>
-      <c r="HN1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN29</t>
-        </is>
-      </c>
-      <c r="HO1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN29</t>
-        </is>
-      </c>
-      <c r="HP1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN30</t>
-        </is>
-      </c>
-      <c r="HQ1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN30</t>
-        </is>
-      </c>
-      <c r="HR1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN30</t>
-        </is>
-      </c>
-      <c r="HS1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN30</t>
-        </is>
-      </c>
-      <c r="HT1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN30</t>
-        </is>
-      </c>
-      <c r="HU1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN31</t>
-        </is>
-      </c>
-      <c r="HV1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN31</t>
-        </is>
-      </c>
-      <c r="HW1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN31</t>
-        </is>
-      </c>
-      <c r="HX1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN31</t>
-        </is>
-      </c>
-      <c r="HY1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN31</t>
-        </is>
-      </c>
-      <c r="HZ1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN32</t>
-        </is>
-      </c>
-      <c r="IA1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN32</t>
-        </is>
-      </c>
-      <c r="IB1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN32</t>
-        </is>
-      </c>
-      <c r="IC1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN32</t>
-        </is>
-      </c>
-      <c r="ID1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN32</t>
-        </is>
-      </c>
-      <c r="IE1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN33</t>
-        </is>
-      </c>
-      <c r="IF1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN33</t>
-        </is>
-      </c>
-      <c r="IG1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN33</t>
-        </is>
-      </c>
-      <c r="IH1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN33</t>
-        </is>
-      </c>
-      <c r="II1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN33</t>
-        </is>
-      </c>
-      <c r="IJ1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN34</t>
-        </is>
-      </c>
-      <c r="IK1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN34</t>
-        </is>
-      </c>
-      <c r="IL1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN34</t>
-        </is>
-      </c>
-      <c r="IM1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN34</t>
-        </is>
-      </c>
-      <c r="IN1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN34</t>
-        </is>
-      </c>
-      <c r="IO1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN35</t>
-        </is>
-      </c>
-      <c r="IP1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN35</t>
-        </is>
-      </c>
-      <c r="IQ1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN35</t>
-        </is>
-      </c>
-      <c r="IR1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN35</t>
-        </is>
-      </c>
-      <c r="IS1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN35</t>
-        </is>
-      </c>
-      <c r="IT1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN36</t>
-        </is>
-      </c>
-      <c r="IU1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN36</t>
-        </is>
-      </c>
-      <c r="IV1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN36</t>
-        </is>
-      </c>
-      <c r="IW1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN36</t>
-        </is>
-      </c>
-      <c r="IX1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN36</t>
-        </is>
-      </c>
-      <c r="IY1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN37</t>
-        </is>
-      </c>
-      <c r="IZ1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN37</t>
-        </is>
-      </c>
-      <c r="JA1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN37</t>
-        </is>
-      </c>
-      <c r="JB1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN37</t>
-        </is>
-      </c>
-      <c r="JC1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN37</t>
-        </is>
-      </c>
-      <c r="JD1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN38</t>
-        </is>
-      </c>
-      <c r="JE1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN38</t>
-        </is>
-      </c>
-      <c r="JF1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN38</t>
-        </is>
-      </c>
-      <c r="JG1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN38</t>
-        </is>
-      </c>
-      <c r="JH1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN38</t>
-        </is>
-      </c>
-      <c r="JI1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN39</t>
-        </is>
-      </c>
-      <c r="JJ1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN39</t>
-        </is>
-      </c>
-      <c r="JK1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN39</t>
-        </is>
-      </c>
-      <c r="JL1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN39</t>
-        </is>
-      </c>
-      <c r="JM1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN39</t>
-        </is>
-      </c>
-      <c r="JN1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN40</t>
-        </is>
-      </c>
-      <c r="JO1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN40</t>
-        </is>
-      </c>
-      <c r="JP1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN40</t>
-        </is>
-      </c>
-      <c r="JQ1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN40</t>
-        </is>
-      </c>
-      <c r="JR1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN40</t>
-        </is>
-      </c>
-      <c r="JS1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MEAN)//INTENSITY//SHELL_EDGE_PROFILE_BIN41</t>
-        </is>
-      </c>
-      <c r="JT1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MIN)//INTENSITY//SHELL_EDGE_PROFILE_BIN41</t>
-        </is>
-      </c>
-      <c r="JU1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_MAX)//INTENSITY//SHELL_EDGE_PROFILE_BIN41</t>
-        </is>
-      </c>
-      <c r="JV1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_STD)//INTENSITY//SHELL_EDGE_PROFILE_BIN41</t>
-        </is>
-      </c>
-      <c r="JW1" t="inlineStr">
-        <is>
-          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN41</t>
+          <t>SPHERE_(OBJ_SUM)//INTENSITY//SHELL_EDGE_PROFILE_BIN41_(15.00PX)</t>
         </is>
       </c>
     </row>
@@ -2407,6 +2015,12 @@
       <c r="D2" t="n">
         <v>0.0</v>
       </c>
+      <c r="E2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>4.9E-324</v>
+      </c>
       <c r="G2" t="e">
         <v>#NUM!</v>
       </c>
@@ -2416,6 +2030,12 @@
       <c r="I2" t="n">
         <v>0.0</v>
       </c>
+      <c r="J2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>4.9E-324</v>
+      </c>
       <c r="L2" t="e">
         <v>#NUM!</v>
       </c>
@@ -2423,17 +2043,29 @@
         <v>0.0</v>
       </c>
       <c r="N2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="P2" t="n">
         <v>4.9E-324</v>
       </c>
       <c r="Q2" t="e">
         <v>#NUM!</v>
       </c>
       <c r="R2" t="n">
-        <v>4.9E-324</v>
+        <v>0.0</v>
       </c>
       <c r="S2" t="n">
         <v>0.0</v>
       </c>
+      <c r="T2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="U2" t="n">
+        <v>4.9E-324</v>
+      </c>
       <c r="V2" t="e">
         <v>#NUM!</v>
       </c>
@@ -2443,114 +2075,192 @@
       <c r="X2" t="n">
         <v>0.0</v>
       </c>
+      <c r="Y2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="Z2" t="n">
+        <v>4.9E-324</v>
+      </c>
       <c r="AA2" t="e">
         <v>#NUM!</v>
       </c>
       <c r="AB2" t="n">
         <v>0.0</v>
       </c>
-      <c r="AC2" t="e">
-        <v>#NUM!</v>
+      <c r="AC2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AD2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AE2" t="n">
+        <v>4.9E-324</v>
       </c>
       <c r="AF2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="AG2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="AH2" t="e">
-        <v>#NUM!</v>
+      <c r="AG2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AH2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AI2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AJ2" t="n">
+        <v>4.9E-324</v>
       </c>
       <c r="AK2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="AL2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="AM2" t="e">
-        <v>#NUM!</v>
+      <c r="AL2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AM2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AO2" t="n">
+        <v>4.9E-324</v>
       </c>
       <c r="AP2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="AQ2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="AR2" t="e">
-        <v>#NUM!</v>
+      <c r="AQ2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AR2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AS2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AT2" t="n">
+        <v>4.9E-324</v>
       </c>
       <c r="AU2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="AV2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="AW2" t="e">
-        <v>#NUM!</v>
+      <c r="AV2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AW2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AX2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="AY2" t="n">
+        <v>4.9E-324</v>
       </c>
       <c r="AZ2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="BA2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="BB2" t="e">
-        <v>#NUM!</v>
+      <c r="BA2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BB2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BC2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BD2" t="n">
+        <v>4.9E-324</v>
       </c>
       <c r="BE2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="BF2" t="e">
-        <v>#NUM!</v>
+      <c r="BF2" t="n">
+        <v>0.0</v>
       </c>
       <c r="BG2" t="n">
-        <v>10.143835675226494</v>
+        <v>0.0</v>
+      </c>
+      <c r="BH2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BI2" t="n">
+        <v>4.9E-324</v>
       </c>
       <c r="BJ2" t="e">
         <v>#NUM!</v>
       </c>
       <c r="BK2" t="n">
-        <v>10.143835675226494</v>
+        <v>0.0</v>
       </c>
       <c r="BL2" t="n">
-        <v>0.2028767135045299</v>
+        <v>0.0</v>
+      </c>
+      <c r="BM2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BN2" t="n">
+        <v>4.9E-324</v>
       </c>
       <c r="BO2" t="e">
         <v>#NUM!</v>
       </c>
       <c r="BP2" t="n">
-        <v>0.2028767135045299</v>
+        <v>0.0</v>
       </c>
       <c r="BQ2" t="n">
-        <v>0.23663051323649173</v>
+        <v>0.0</v>
+      </c>
+      <c r="BR2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BS2" t="n">
+        <v>4.9E-324</v>
       </c>
       <c r="BT2" t="e">
         <v>#NUM!</v>
       </c>
       <c r="BU2" t="n">
-        <v>0.23663051323649173</v>
+        <v>0.0</v>
       </c>
       <c r="BV2" t="n">
-        <v>0.004732610264729834</v>
+        <v>0.0</v>
+      </c>
+      <c r="BW2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="BX2" t="n">
+        <v>4.9E-324</v>
       </c>
       <c r="BY2" t="e">
         <v>#NUM!</v>
       </c>
       <c r="BZ2" t="n">
-        <v>0.004732610264729834</v>
-      </c>
-      <c r="CA2" t="e">
-        <v>#NUM!</v>
+        <v>0.0</v>
+      </c>
+      <c r="CA2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="CB2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="CC2" t="n">
+        <v>4.9E-324</v>
       </c>
       <c r="CD2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="CE2" t="e">
-        <v>#NUM!</v>
+      <c r="CE2" t="n">
+        <v>0.0</v>
       </c>
       <c r="CF2" t="n">
         <v>0.0</v>
       </c>
+      <c r="CG2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="CH2" t="n">
+        <v>4.9E-324</v>
+      </c>
       <c r="CI2" t="e">
         <v>#NUM!</v>
       </c>
@@ -2560,6 +2270,12 @@
       <c r="CK2" t="n">
         <v>0.0</v>
       </c>
+      <c r="CL2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="CM2" t="n">
+        <v>4.9E-324</v>
+      </c>
       <c r="CN2" t="e">
         <v>#NUM!</v>
       </c>
@@ -2569,6 +2285,12 @@
       <c r="CP2" t="n">
         <v>0.0</v>
       </c>
+      <c r="CQ2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="CR2" t="n">
+        <v>4.9E-324</v>
+      </c>
       <c r="CS2" t="e">
         <v>#NUM!</v>
       </c>
@@ -2576,17 +2298,29 @@
         <v>0.0</v>
       </c>
       <c r="CU2" t="n">
-        <v>0.0</v>
+        <v>101.35983263598321</v>
+      </c>
+      <c r="CV2" t="n">
+        <v>101.35983263598321</v>
+      </c>
+      <c r="CW2" t="n">
+        <v>101.35983263598321</v>
       </c>
       <c r="CX2" t="e">
         <v>#NUM!</v>
       </c>
       <c r="CY2" t="n">
-        <v>0.0</v>
+        <v>101.35983263598321</v>
       </c>
       <c r="CZ2" t="n">
         <v>0.0</v>
       </c>
+      <c r="DA2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="DB2" t="n">
+        <v>4.9E-324</v>
+      </c>
       <c r="DC2" t="e">
         <v>#NUM!</v>
       </c>
@@ -2596,6 +2330,12 @@
       <c r="DE2" t="n">
         <v>0.0</v>
       </c>
+      <c r="DF2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="DG2" t="n">
+        <v>4.9E-324</v>
+      </c>
       <c r="DH2" t="e">
         <v>#NUM!</v>
       </c>
@@ -2605,6 +2345,12 @@
       <c r="DJ2" t="n">
         <v>0.0</v>
       </c>
+      <c r="DK2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="DL2" t="n">
+        <v>4.9E-324</v>
+      </c>
       <c r="DM2" t="e">
         <v>#NUM!</v>
       </c>
@@ -2614,6 +2360,12 @@
       <c r="DO2" t="n">
         <v>0.0</v>
       </c>
+      <c r="DP2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="DQ2" t="n">
+        <v>4.9E-324</v>
+      </c>
       <c r="DR2" t="e">
         <v>#NUM!</v>
       </c>
@@ -2623,6 +2375,12 @@
       <c r="DT2" t="n">
         <v>0.0</v>
       </c>
+      <c r="DU2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="DV2" t="n">
+        <v>4.9E-324</v>
+      </c>
       <c r="DW2" t="e">
         <v>#NUM!</v>
       </c>
@@ -2632,6 +2390,12 @@
       <c r="DY2" t="n">
         <v>0.0</v>
       </c>
+      <c r="DZ2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="EA2" t="n">
+        <v>4.9E-324</v>
+      </c>
       <c r="EB2" t="e">
         <v>#NUM!</v>
       </c>
@@ -2641,6 +2405,12 @@
       <c r="ED2" t="n">
         <v>0.0</v>
       </c>
+      <c r="EE2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="EF2" t="n">
+        <v>4.9E-324</v>
+      </c>
       <c r="EG2" t="e">
         <v>#NUM!</v>
       </c>
@@ -2650,6 +2420,12 @@
       <c r="EI2" t="n">
         <v>0.0</v>
       </c>
+      <c r="EJ2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="EK2" t="n">
+        <v>4.9E-324</v>
+      </c>
       <c r="EL2" t="e">
         <v>#NUM!</v>
       </c>
@@ -2659,6 +2435,12 @@
       <c r="EN2" t="n">
         <v>0.0</v>
       </c>
+      <c r="EO2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="EP2" t="n">
+        <v>4.9E-324</v>
+      </c>
       <c r="EQ2" t="e">
         <v>#NUM!</v>
       </c>
@@ -2668,6 +2450,12 @@
       <c r="ES2" t="n">
         <v>0.0</v>
       </c>
+      <c r="ET2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="EU2" t="n">
+        <v>4.9E-324</v>
+      </c>
       <c r="EV2" t="e">
         <v>#NUM!</v>
       </c>
@@ -2677,6 +2465,12 @@
       <c r="EX2" t="n">
         <v>0.0</v>
       </c>
+      <c r="EY2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="EZ2" t="n">
+        <v>4.9E-324</v>
+      </c>
       <c r="FA2" t="e">
         <v>#NUM!</v>
       </c>
@@ -2686,6 +2480,12 @@
       <c r="FC2" t="n">
         <v>0.0</v>
       </c>
+      <c r="FD2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="FE2" t="n">
+        <v>4.9E-324</v>
+      </c>
       <c r="FF2" t="e">
         <v>#NUM!</v>
       </c>
@@ -2695,6 +2495,12 @@
       <c r="FH2" t="n">
         <v>0.0</v>
       </c>
+      <c r="FI2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="FJ2" t="n">
+        <v>4.9E-324</v>
+      </c>
       <c r="FK2" t="e">
         <v>#NUM!</v>
       </c>
@@ -2702,35 +2508,59 @@
         <v>0.0</v>
       </c>
       <c r="FM2" t="n">
-        <v>0.0</v>
+        <v>31.384615384615458</v>
+      </c>
+      <c r="FN2" t="n">
+        <v>31.384615384615458</v>
+      </c>
+      <c r="FO2" t="n">
+        <v>31.384615384615458</v>
       </c>
       <c r="FP2" t="e">
         <v>#NUM!</v>
       </c>
       <c r="FQ2" t="n">
-        <v>0.0</v>
+        <v>31.384615384615458</v>
       </c>
       <c r="FR2" t="n">
-        <v>0.0</v>
+        <v>13.387500000000008</v>
+      </c>
+      <c r="FS2" t="n">
+        <v>13.387500000000008</v>
+      </c>
+      <c r="FT2" t="n">
+        <v>13.387500000000008</v>
       </c>
       <c r="FU2" t="e">
         <v>#NUM!</v>
       </c>
       <c r="FV2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="FW2" t="e">
-        <v>#NUM!</v>
+        <v>13.387500000000008</v>
+      </c>
+      <c r="FW2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="FX2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="FY2" t="n">
+        <v>4.9E-324</v>
       </c>
       <c r="FZ2" t="e">
         <v>#NUM!</v>
       </c>
-      <c r="GA2" t="e">
-        <v>#NUM!</v>
+      <c r="GA2" t="n">
+        <v>0.0</v>
       </c>
       <c r="GB2" t="n">
         <v>0.0</v>
       </c>
+      <c r="GC2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="GD2" t="n">
+        <v>4.9E-324</v>
+      </c>
       <c r="GE2" t="e">
         <v>#NUM!</v>
       </c>
@@ -2740,6 +2570,12 @@
       <c r="GG2" t="n">
         <v>0.0</v>
       </c>
+      <c r="GH2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="GI2" t="n">
+        <v>4.9E-324</v>
+      </c>
       <c r="GJ2" t="e">
         <v>#NUM!</v>
       </c>
@@ -2749,6 +2585,12 @@
       <c r="GL2" t="n">
         <v>0.0</v>
       </c>
+      <c r="GM2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="GN2" t="n">
+        <v>4.9E-324</v>
+      </c>
       <c r="GO2" t="e">
         <v>#NUM!</v>
       </c>
@@ -2758,6 +2600,12 @@
       <c r="GQ2" t="n">
         <v>0.0</v>
       </c>
+      <c r="GR2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="GS2" t="n">
+        <v>4.9E-324</v>
+      </c>
       <c r="GT2" t="e">
         <v>#NUM!</v>
       </c>
@@ -2767,145 +2615,16 @@
       <c r="GV2" t="n">
         <v>0.0</v>
       </c>
+      <c r="GW2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="GX2" t="n">
+        <v>4.9E-324</v>
+      </c>
       <c r="GY2" t="e">
         <v>#NUM!</v>
       </c>
       <c r="GZ2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="HA2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="HD2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="HE2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="HF2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="HI2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="HJ2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="HK2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="HN2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="HO2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="HP2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="HS2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="HT2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="HU2" t="n">
-        <v>25.31476997578695</v>
-      </c>
-      <c r="HX2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="HY2" t="n">
-        <v>25.31476997578695</v>
-      </c>
-      <c r="HZ2" t="n">
-        <v>5.710808179162615</v>
-      </c>
-      <c r="IC2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="ID2" t="n">
-        <v>5.710808179162615</v>
-      </c>
-      <c r="IE2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="IH2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="II2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="IJ2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="IM2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="IN2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="IO2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="IR2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="IS2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="IT2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="IW2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="IX2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="IY2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="JB2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="JC2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="JD2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="JG2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="JH2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="JI2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="JL2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="JM2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="JN2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="JQ2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="JR2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="JS2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="JV2" t="e">
-        <v>#NUM!</v>
-      </c>
-      <c r="JW2" t="n">
         <v>0.0</v>
       </c>
     </row>
@@ -2945,282 +2664,207 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_MEAN</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN01_(-15.00PX)</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_MIN</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN02_(-14.25PX)</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_MAX</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN03_(-13.50PX)</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_STDEV</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN04_(-12.75PX)</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_SUM</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN05_(-12.00PX)</t>
         </is>
       </c>
       <c r="J1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_X_CENTRE_MEAN (PX)</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN06_(-11.25PX)</t>
         </is>
       </c>
       <c r="K1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_X_CENTRE_STDEV (PX)</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN07_(-10.50PX)</t>
         </is>
       </c>
       <c r="L1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_Y_CENTRE_MEAN (PX)</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN08_(-9.75PX)</t>
         </is>
       </c>
       <c r="M1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_Y_CENTRE_STDEV (PX)</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN09_(-9.00PX)</t>
         </is>
       </c>
       <c r="N1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_Z_CENTRE_MEAN (SLICE)</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN10_(-8.25PX)</t>
         </is>
       </c>
       <c r="O1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_Z_CENTRE_STDEV (SLICE)</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN11_(-7.50PX)</t>
         </is>
       </c>
       <c r="P1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_MEAN_EDGE_DISTANCE (PX)</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN12_(-6.75PX)</t>
         </is>
       </c>
       <c r="Q1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_MEAN_EDGE_DISTANCE (CAL)</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN13_(-6.00PX)</t>
         </is>
       </c>
       <c r="R1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_STD_EDGE_DISTANCE (PX)</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN14_(-5.25PX)</t>
         </is>
       </c>
       <c r="S1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_STD_EDGE_DISTANCE (CAL)</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN15_(-4.50PX)</t>
         </is>
       </c>
       <c r="T1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN1</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN16_(-3.75PX)</t>
         </is>
       </c>
       <c r="U1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN2</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN17_(-3.00PX)</t>
         </is>
       </c>
       <c r="V1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN3</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN18_(-2.25PX)</t>
         </is>
       </c>
       <c r="W1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN4</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN19_(-1.50PX)</t>
         </is>
       </c>
       <c r="X1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN5</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN20_(-.75PX)</t>
         </is>
       </c>
       <c r="Y1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN6</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN21_(.00PX)</t>
         </is>
       </c>
       <c r="Z1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN7</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN22_(.75PX)</t>
         </is>
       </c>
       <c r="AA1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN8</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN23_(1.50PX)</t>
         </is>
       </c>
       <c r="AB1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN9</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN24_(2.25PX)</t>
         </is>
       </c>
       <c r="AC1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN10</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN25_(3.00PX)</t>
         </is>
       </c>
       <c r="AD1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN11</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN26_(3.75PX)</t>
         </is>
       </c>
       <c r="AE1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN12</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN27_(4.50PX)</t>
         </is>
       </c>
       <c r="AF1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN13</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN28_(5.25PX)</t>
         </is>
       </c>
       <c r="AG1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN14</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN29_(6.00PX)</t>
         </is>
       </c>
       <c r="AH1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN15</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN30_(6.75PX)</t>
         </is>
       </c>
       <c r="AI1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN16</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN31_(7.50PX)</t>
         </is>
       </c>
       <c r="AJ1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN17</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN32_(8.25PX)</t>
         </is>
       </c>
       <c r="AK1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN18</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN33_(9.00PX)</t>
         </is>
       </c>
       <c r="AL1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN19</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN34_(9.75PX)</t>
         </is>
       </c>
       <c r="AM1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN20</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN35_(10.50PX)</t>
         </is>
       </c>
       <c r="AN1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN21</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN36_(11.25PX)</t>
         </is>
       </c>
       <c r="AO1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN22</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN37_(12.00PX)</t>
         </is>
       </c>
       <c r="AP1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN23</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN38_(12.75PX)</t>
         </is>
       </c>
       <c r="AQ1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN24</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN39_(13.50PX)</t>
         </is>
       </c>
       <c r="AR1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN25</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN40_(14.25PX)</t>
         </is>
       </c>
       <c r="AS1" t="inlineStr">
         <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN26</t>
-        </is>
-      </c>
-      <c r="AT1" t="inlineStr">
-        <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN27</t>
-        </is>
-      </c>
-      <c r="AU1" t="inlineStr">
-        <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN28</t>
-        </is>
-      </c>
-      <c r="AV1" t="inlineStr">
-        <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN29</t>
-        </is>
-      </c>
-      <c r="AW1" t="inlineStr">
-        <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN30</t>
-        </is>
-      </c>
-      <c r="AX1" t="inlineStr">
-        <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN31</t>
-        </is>
-      </c>
-      <c r="AY1" t="inlineStr">
-        <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN32</t>
-        </is>
-      </c>
-      <c r="AZ1" t="inlineStr">
-        <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN33</t>
-        </is>
-      </c>
-      <c r="BA1" t="inlineStr">
-        <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN34</t>
-        </is>
-      </c>
-      <c r="BB1" t="inlineStr">
-        <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN35</t>
-        </is>
-      </c>
-      <c r="BC1" t="inlineStr">
-        <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN36</t>
-        </is>
-      </c>
-      <c r="BD1" t="inlineStr">
-        <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN37</t>
-        </is>
-      </c>
-      <c r="BE1" t="inlineStr">
-        <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN38</t>
-        </is>
-      </c>
-      <c r="BF1" t="inlineStr">
-        <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN39</t>
-        </is>
-      </c>
-      <c r="BG1" t="inlineStr">
-        <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN40</t>
-        </is>
-      </c>
-      <c r="BH1" t="inlineStr">
-        <is>
-          <t>INTENSITY//Shell_EDGE_PROFILE_BIN41</t>
+          <t>INTENSITY//Shell_EDGE_PROFILE_BIN41_(15.00PX)</t>
         </is>
       </c>
     </row>
@@ -3248,7 +2892,7 @@
         <v>0.0</v>
       </c>
       <c r="G2" t="n">
-        <v>4.9E-324</v>
+        <v>0.0</v>
       </c>
       <c r="H2" t="n">
         <v>0.0</v>
@@ -3256,52 +2900,38 @@
       <c r="I2" t="n">
         <v>0.0</v>
       </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="N2" t="inlineStr">
-        <is>
-          <t/>
-        </is>
-      </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+      <c r="J2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="K2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="L2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="N2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="O2" t="n">
+        <v>0.0</v>
       </c>
       <c r="P2" t="n">
-        <v>10.143835675226494</v>
+        <v>0.0</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.2028767135045299</v>
+        <v>0.0</v>
       </c>
       <c r="R2" t="n">
-        <v>0.23663051323649173</v>
+        <v>0.0</v>
       </c>
       <c r="S2" t="n">
-        <v>0.004732610264729834</v>
-      </c>
-      <c r="T2" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+        <v>0.0</v>
+      </c>
+      <c r="T2" t="n">
+        <v>0.0</v>
       </c>
       <c r="U2" t="n">
         <v>0.0</v>
@@ -3313,7 +2943,7 @@
         <v>0.0</v>
       </c>
       <c r="X2" t="n">
-        <v>0.0</v>
+        <v>101.35983263598321</v>
       </c>
       <c r="Y2" t="n">
         <v>0.0</v>
@@ -3355,15 +2985,13 @@
         <v>0.0</v>
       </c>
       <c r="AL2" t="n">
-        <v>0.0</v>
+        <v>31.384615384615458</v>
       </c>
       <c r="AM2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AN2" t="inlineStr">
-        <is>
-          <t/>
-        </is>
+        <v>13.387500000000008</v>
+      </c>
+      <c r="AN2" t="n">
+        <v>0.0</v>
       </c>
       <c r="AO2" t="n">
         <v>0.0</v>
@@ -3378,51 +3006,6 @@
         <v>0.0</v>
       </c>
       <c r="AS2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AT2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AU2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AV2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AW2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="AX2" t="n">
-        <v>25.31476997578695</v>
-      </c>
-      <c r="AY2" t="n">
-        <v>5.710808179162615</v>
-      </c>
-      <c r="AZ2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="BA2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="BB2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="BC2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="BD2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="BE2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="BF2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="BG2" t="n">
-        <v>0.0</v>
-      </c>
-      <c r="BH2" t="n">
         <v>0.0</v>
       </c>
     </row>

</xml_diff>